<commit_message>
Fix datasources in demo SpOTy
</commit_message>
<xml_diff>
--- a/demos/demo-SpOTy/sparnatural-config.xlsx
+++ b/demos/demo-SpOTy/sparnatural-config.xlsx
@@ -4,7 +4,7 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="0">#REF!</definedName>
   </definedNames>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
@@ -1359,7 +1362,7 @@
   </si>
   <si>
     <t xml:space="preserve">PREFIX skos: &lt;http://www.w3.org/2004/02/skos/core#&gt;
-PREFIX spoty: &lt;https://aslan.universite-lyon.fr/spoty/ns/&gt;
+PREFIX spoty: &lt;https://w3id.org/SpOTy/ontology#&gt;
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 SELECT DISTINCT ?uri (concat(?code, " ", ?lbl) as ?label)
 WHERE {
@@ -1368,13 +1371,12 @@
     spoty:code ?code .
  FILTER(isIRI(?uri))
  FILTER(lang(?lbl) = $lang)
- BIND(bound(?child) AS ?hasChildren)
 }
 ORDER BY UCASE(?label)</t>
   </si>
   <si>
     <t xml:space="preserve">PREFIX skos: &lt;http://www.w3.org/2004/02/skos/core#&gt;
-PREFIX spoty: &lt;https://aslan.universite-lyon.fr/spoty/ns/&gt;
+PREFIX spoty: &lt;https://w3id.org/SpOTy/ontology#&gt;
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 SELECT DISTINCT ?uri (concat(?code, " ", ?lbl) as ?label) ?hasChildren
 WHERE {
@@ -1395,7 +1397,7 @@
     <t>this:search_language</t>
   </si>
   <si>
-    <t xml:space="preserve">PREFIX spoty: &lt;https://aslan.universite-lyon.fr/spoty/ns/&gt;
+    <t xml:space="preserve">PREFIX spoty: &lt;https://w3id.org/SpOTy/ontology#&gt;
     PREFIX wdt: &lt;http://www.wikidata.org/prop/direct/&gt;
     PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
     SELECT DISTINCT ?uri ?label {
@@ -2551,7 +2553,7 @@
     </xf>
     <xf fontId="13" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2795,6 +2797,10 @@
     </xf>
     <xf fontId="32" fillId="51" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
+      <alignment wrapText="1"/>
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="32" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right"/>
@@ -3774,7 +3780,7 @@
     <hyperlink r:id="rId17" ref="C18"/>
     <hyperlink r:id="rId18" ref="C19"/>
     <hyperlink r:id="rId19" ref="C20"/>
-    <hyperlink r:id="rId20" ref="C21" tooltip=""/>
+    <hyperlink r:id="rId20" ref="C21"/>
     <hyperlink r:id="rId21" ref="C22"/>
     <hyperlink r:id="rId22" ref="C23"/>
     <hyperlink r:id="rId23" ref="C24"/>
@@ -8641,7 +8647,7 @@
       <c r="B6" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="79" t="s">
         <v>417</v>
       </c>
       <c r="D6" s="12"/>
@@ -8653,7 +8659,7 @@
       <c r="B7" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="79" t="s">
         <v>418</v>
       </c>
       <c r="D7" s="12"/>
@@ -8665,7 +8671,7 @@
       <c r="B8" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="79" t="s">
         <v>420</v>
       </c>
       <c r="D8" s="12"/>
@@ -8677,7 +8683,7 @@
       <c r="B9" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="79" t="s">
         <v>421</v>
       </c>
       <c r="D9" s="12"/>
@@ -8706,31 +8712,31 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="80" t="str">
+      <c r="B1" s="81" t="str">
         <f>Entities!B1</f>
         <v>https://w3id.org/SpOTy/shapes-ldo</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="82" t="s">
         <v>164</v>
       </c>
       <c r="D1" s="46"/>
-      <c r="E1" s="81"/>
+      <c r="E1" s="82"/>
       <c r="F1" s="46"/>
       <c r="G1" s="46"/>
       <c r="H1" s="46"/>
       <c r="I1" s="46"/>
     </row>
     <row r="2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="80" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>422</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>423</v>
       </c>
       <c r="D2" s="46"/>
@@ -8752,21 +8758,21 @@
       <c r="I3" s="46"/>
     </row>
     <row r="4">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>424</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8874,13 +8880,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>428</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="86" t="s">
         <v>429</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="86" t="s">
         <v>430</v>
       </c>
     </row>

</xml_diff>